<commit_message>
WIP training with examtopics.com
</commit_message>
<xml_diff>
--- a/1z0-809_topic.xlsx
+++ b/1z0-809_topic.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hirokiinoue/git_repositories/EXAM_1Z0-809/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a859432\git_repository\EXAM_1Z0-809\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07651AC0-860A-3543-85B8-6307597DBCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE617B4-5D70-4D65-A429-77A3FA95C493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17000" xr2:uid="{956B1D0D-F1A3-6146-85C0-0D84789ECF4C}"/>
+    <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" activeTab="1" xr2:uid="{956B1D0D-F1A3-6146-85C0-0D84789ECF4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="examtopics.com Q1" sheetId="2" r:id="rId2"/>
+    <sheet name="examtopis.com Q2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>1.1</t>
   </si>
@@ -230,40 +232,46 @@
     <t>Description</t>
   </si>
   <si>
-    <t>1. Design Patterns and Principles</t>
-  </si>
-  <si>
-    <t>2. Advanced Class Design</t>
-  </si>
-  <si>
-    <t>3. Generics and Collections</t>
-  </si>
-  <si>
-    <t>7. Exception and Assertions</t>
-  </si>
-  <si>
-    <t>8. Dates</t>
-  </si>
-  <si>
-    <t>10. NIO.2</t>
-  </si>
-  <si>
-    <t>11. Concurrency</t>
-  </si>
-  <si>
-    <t>12. JDBC</t>
-  </si>
-  <si>
-    <t>13. Localization</t>
-  </si>
-  <si>
-    <t>4. Functional Programming()</t>
-  </si>
-  <si>
-    <t>5. Functional Programming()</t>
-  </si>
-  <si>
-    <t>6. Functional Programming()</t>
+    <t>?</t>
+  </si>
+  <si>
+    <t>12. JDBC (Chapter 10)</t>
+  </si>
+  <si>
+    <t>13. Localization (Chapter 5)</t>
+  </si>
+  <si>
+    <t>11. Concurrency (Chapter 7)</t>
+  </si>
+  <si>
+    <t>10. NIO.2 (Chpater 9)</t>
+  </si>
+  <si>
+    <t>8. Dates (Chapter 5)</t>
+  </si>
+  <si>
+    <t>7. Exception and Assertions (Chapter 6)</t>
+  </si>
+  <si>
+    <t>3. Generics and Collections (Chapter 3)</t>
+  </si>
+  <si>
+    <t>4. Functional Programming (Chpter 4)</t>
+  </si>
+  <si>
+    <t>5. Functional Programming (Chapter 4)</t>
+  </si>
+  <si>
+    <t>6. Functional Programming (Chapter 4)</t>
+  </si>
+  <si>
+    <t>2. Advanced Class Design (Chapter 1)</t>
+  </si>
+  <si>
+    <t>1. Design Patterns and Principles (Chapter 2)</t>
+  </si>
+  <si>
+    <t>penso che fosse una domanda simile come la domanda 2 di examtopics.</t>
   </si>
 </sst>
 </file>
@@ -351,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -360,17 +368,23 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -387,6 +401,438 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>580008</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>65917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6B3FF9-5BBF-50B2-6C64-637AC8E5F71C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="7600950"/>
+          <a:ext cx="8133333" cy="6066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>608581</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>75465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBFD85D9-3488-DEC6-967D-8901A7FCA1E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="200025"/>
+          <a:ext cx="8152381" cy="5876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{266F3C56-BD20-1E16-7B53-B65E1B5FC887}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="6200775"/>
+          <a:ext cx="8134350" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A. Velocity with new speed 1 kmph</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>B. A compilation error occurs at line n1.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>C. A compilation error occurs at line n2.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>D. A compilation error occurs at line n3.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>618019</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>37720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{180DE975-5EB8-4A48-495B-32BDE61CB27D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="7600950"/>
+          <a:ext cx="8847619" cy="3038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>522952</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85364</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC677B2B-4A86-A2B4-192F-757E835D07F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="400050"/>
+          <a:ext cx="7380952" cy="2885714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9184D0CD-41DF-4809-1753-D7B1767D74FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695324" y="3657600"/>
+          <a:ext cx="7343775" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A. Replace line n1 with: IntFunction&lt;UnaryOperator&gt; inFu = x -&gt; y -&gt; x*y;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>B. Replace line n1 with: IntFunction&lt;IntUnaryOperator&gt; inFu = x -&gt; y -&gt; x*y;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>C. Replace line n1 with: BiFunction&lt;IntUnaryOperator&gt; inFu = x -&gt; y -&gt; x*y;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>D. Replace line n2 with: IntStream newStream = stream.map(inFu.applyAsInt (10));</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,443 +1134,451 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B7CF54-6BEF-A946-BB5E-88E53BF8D10B}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="164" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="117.875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>64</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>65</v>
+    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>66</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>73</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>74</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>75</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>67</v>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>68</v>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="4"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>69</v>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>70</v>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>71</v>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="4"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
+    <row r="37" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>72</v>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D40" s="1"/>
@@ -1145,4 +1599,34 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6577BFF-F115-49CB-A2FB-1D7DE9D330E9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56B1680-7189-43F5-BFD0-F5E8F22F8F8C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>